<commit_message>
se actualizo la lista de comandos
</commit_message>
<xml_diff>
--- a/comandos.xlsx
+++ b/comandos.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$51</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -584,10 +584,10 @@
     <t xml:space="preserve">git commit -a  </t>
   </si>
   <si>
-    <t>me manda a VIM - este comando es como hacer el git add pero me envia a vim prahacer el comentario del commit</t>
-  </si>
-  <si>
     <t>es como hacer git add y git commit -m " " a la vez</t>
+  </si>
+  <si>
+    <t>me manda a VIM - este comando es como hacer el git add pero me envia a vim prahacer el comentario del commit (a) de add y (m) de mansaje</t>
   </si>
 </sst>
 </file>
@@ -1872,10 +1872,10 @@
   <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B46" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A51" sqref="A51"/>
+      <selection pane="bottomRight" activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2275,19 +2275,18 @@
         <v>90</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C50"/>
   <mergeCells count="1">
     <mergeCell ref="A7:A8"/>
   </mergeCells>

</xml_diff>